<commit_message>
Update cost option 4
</commit_message>
<xml_diff>
--- a/Board3 - Shorty/Documents/Board3 BOM.xlsx
+++ b/Board3 - Shorty/Documents/Board3 BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AA2B12-2E52-4A0A-800A-9C9C9E69890E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261AD875-574B-4C59-A34F-3FD17432DD08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1242,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R47"/>
+  <dimension ref="A2:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1485,8 +1485,8 @@
         <v>4</v>
       </c>
       <c r="Q10" s="29">
-        <f>5*SUM(J9:J18,J23,J29:J36)+SUM(J38:J40,J42)+77+J47</f>
-        <v>219.75</v>
+        <f>5*SUM(J7:J18,J23,J29:J36)+SUM(J38:J40,J42)+J37+J41+J24+77+J47</f>
+        <v>294.89</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>167</v>
@@ -2491,6 +2491,11 @@
       </c>
       <c r="J47" s="6">
         <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9">
+      <c r="I52" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Cyclone Rocketry Logo, generate gerbers
</commit_message>
<xml_diff>
--- a/Board3 - Shorty/Documents/Board3 BOM.xlsx
+++ b/Board3 - Shorty/Documents/Board3 BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261AD875-574B-4C59-A34F-3FD17432DD08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FA97A1-40A2-4CA5-A679-6D1745D77715}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
     <t>Cost of PCB</t>
   </si>
   <si>
-    <t>All passives and microcontrollers and sensors installed. No RF or GPS components installed</t>
+    <t>All passives and microcontrollers and sensors installed. LoRa and GPS components installed on one</t>
   </si>
 </sst>
 </file>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1264,7 +1264,7 @@
     <col min="15" max="15" width="9" style="6" customWidth="1"/>
     <col min="16" max="16" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" style="6" customWidth="1"/>
-    <col min="18" max="18" width="92.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="98.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -1485,8 +1485,8 @@
         <v>4</v>
       </c>
       <c r="Q10" s="29">
-        <f>5*SUM(J7:J18,J23,J29:J36)+SUM(J38:J40,J42)+J37+J41+J24+77+J47</f>
-        <v>294.89</v>
+        <f>5*SUM(J9:J18,J23,J29:J36)+SUM(J38:J40,J42)+J37+J41+J24+J8+77+J47</f>
+        <v>270.76</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>167</v>

</xml_diff>